<commit_message>
Functions added: show whole roster, exclude players, other functions added...
</commit_message>
<xml_diff>
--- a/stats.xlsx
+++ b/stats.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e558b79b752fc558/Escritorio/py/lineup/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e558b79b752fc558/Escritorio/py/MLBLineupsGenerator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="293" documentId="8_{8D71F00F-D618-4215-BF17-55F1C2D0446A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{20BF134C-D362-4AFB-8A57-15E510EE54E4}"/>
+  <xr:revisionPtr revIDLastSave="312" documentId="8_{8D71F00F-D618-4215-BF17-55F1C2D0446A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DADEDDEF-877F-4916-80B7-F9305563658F}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{A398CFD0-6192-4D5C-94D1-EAF604C763A7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{A398CFD0-6192-4D5C-94D1-EAF604C763A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3924,8 +3924,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B94100E2-FC9D-4B8A-BC5F-8F3ECDA46C1A}">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection sqref="A1:M19"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="U10" sqref="U10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4003,19 +4003,19 @@
         <v>91</v>
       </c>
       <c r="F2" s="27">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G2" s="28">
         <v>75</v>
       </c>
       <c r="H2" s="28">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I2" s="28">
         <v>40</v>
       </c>
       <c r="J2" s="28">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K2" s="28">
         <v>69</v>
@@ -4024,7 +4024,7 @@
         <v>79</v>
       </c>
       <c r="M2" s="28">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
@@ -4047,7 +4047,7 @@
         <v>98</v>
       </c>
       <c r="G3" s="28">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H3" s="28">
         <v>82</v>
@@ -4056,7 +4056,7 @@
         <v>79</v>
       </c>
       <c r="J3" s="28">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K3" s="28">
         <v>98</v>
@@ -4088,7 +4088,7 @@
         <v>94</v>
       </c>
       <c r="G4" s="28">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H4" s="28">
         <v>89</v>
@@ -4097,7 +4097,7 @@
         <v>50</v>
       </c>
       <c r="J4" s="28">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="K4" s="28">
         <v>85</v>
@@ -4135,7 +4135,7 @@
         <v>99</v>
       </c>
       <c r="I5" s="28">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="J5" s="28">
         <v>99</v>
@@ -4167,13 +4167,13 @@
         <v>76</v>
       </c>
       <c r="F6" s="27">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G6" s="28">
         <v>48</v>
       </c>
       <c r="H6" s="28">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="I6" s="28">
         <v>83</v>
@@ -4229,7 +4229,7 @@
         <v>49</v>
       </c>
       <c r="M7" s="28">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
@@ -4249,7 +4249,7 @@
         <v>78</v>
       </c>
       <c r="F8" s="27">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="G8" s="28">
         <v>44</v>
@@ -4331,7 +4331,7 @@
         <v>68</v>
       </c>
       <c r="F10" s="27">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="G10" s="28">
         <v>60</v>
@@ -4343,7 +4343,7 @@
         <v>48</v>
       </c>
       <c r="J10" s="28">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="K10" s="28">
         <v>77</v>
@@ -4370,7 +4370,7 @@
         <v>2</v>
       </c>
       <c r="E11" s="27">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F11" s="27">
         <v>72</v>
@@ -4379,7 +4379,7 @@
         <v>50</v>
       </c>
       <c r="H11" s="28">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I11" s="28">
         <v>68</v>
@@ -4469,10 +4469,10 @@
         <v>59</v>
       </c>
       <c r="J13" s="28">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K13" s="28">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="L13" s="28">
         <v>45</v>
@@ -4746,8 +4746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8E9409E-4402-4D0B-B853-36FBBCBB5840}">
   <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5517,14 +5517,14 @@
       </c>
       <c r="K5" s="17">
         <f>data_lineup!J3/100</f>
-        <v>0.52</v>
+        <v>0.51</v>
       </c>
       <c r="L5">
         <v>5</v>
       </c>
       <c r="M5">
         <f>L5*K5</f>
-        <v>2.6</v>
+        <v>2.5499999999999998</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
function to excluded 1 player o more of the lineup added
</commit_message>
<xml_diff>
--- a/stats.xlsx
+++ b/stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e558b79b752fc558/Escritorio/py/MLBLineupsGenerator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="312" documentId="8_{8D71F00F-D618-4215-BF17-55F1C2D0446A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DADEDDEF-877F-4916-80B7-F9305563658F}"/>
+  <xr:revisionPtr revIDLastSave="533" documentId="8_{8D71F00F-D618-4215-BF17-55F1C2D0446A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BF8CF7D8-95F5-446E-9E5F-EA59C8CD2B18}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{A398CFD0-6192-4D5C-94D1-EAF604C763A7}"/>
   </bookViews>
@@ -16,9 +16,10 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="data" sheetId="2" r:id="rId2"/>
     <sheet name="Stats montly" sheetId="4" r:id="rId3"/>
-    <sheet name="data_lineup" sheetId="5" r:id="rId4"/>
-    <sheet name="as" sheetId="7" r:id="rId5"/>
-    <sheet name="Sheet4" sheetId="6" r:id="rId6"/>
+    <sheet name="LAA" sheetId="5" r:id="rId4"/>
+    <sheet name="TEX" sheetId="8" r:id="rId5"/>
+    <sheet name="AOK" sheetId="7" r:id="rId6"/>
+    <sheet name="Sheet4" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="158">
   <si>
     <t>Player</t>
   </si>
@@ -479,6 +480,42 @@
   </si>
   <si>
     <t>Lawerence Butler</t>
+  </si>
+  <si>
+    <t>Adolis Garcia</t>
+  </si>
+  <si>
+    <t>Corey Seager</t>
+  </si>
+  <si>
+    <t>Marcus Semien</t>
+  </si>
+  <si>
+    <t>Jonah Heim</t>
+  </si>
+  <si>
+    <t>Josh Jung</t>
+  </si>
+  <si>
+    <t>Mitch Garver</t>
+  </si>
+  <si>
+    <t>Ezequiel Duran</t>
+  </si>
+  <si>
+    <t>Evan carter</t>
+  </si>
+  <si>
+    <t>Leody Taveras</t>
+  </si>
+  <si>
+    <t>Nathaniel Lowe</t>
+  </si>
+  <si>
+    <t>Robie Grossman</t>
+  </si>
+  <si>
+    <t>best hitter</t>
   </si>
 </sst>
 </file>
@@ -3924,8 +3961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B94100E2-FC9D-4B8A-BC5F-8F3ECDA46C1A}">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="U10" sqref="U10"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3940,9 +3977,9 @@
     <col min="9" max="9" width="7.33203125" customWidth="1"/>
     <col min="10" max="10" width="5.77734375" customWidth="1"/>
     <col min="11" max="11" width="7.44140625" customWidth="1"/>
-    <col min="12" max="12" width="6.88671875" customWidth="1"/>
-    <col min="13" max="13" width="9" customWidth="1"/>
-    <col min="14" max="14" width="3.21875" customWidth="1"/>
+    <col min="12" max="12" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.6640625" customWidth="1"/>
+    <col min="14" max="14" width="9.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -4609,7 +4646,7 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="29">
-        <f>data_lineup!A19+1</f>
+        <f>LAA!A19+1</f>
         <v>17</v>
       </c>
       <c r="B17" t="s">
@@ -4693,7 +4730,7 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="29">
-        <f>data_lineup!A16+1</f>
+        <f>LAA!A16+1</f>
         <v>16</v>
       </c>
       <c r="B19" t="s">
@@ -4734,8 +4771,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M15">
-    <sortCondition ref="A2:A15"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="K24:M41">
+    <sortCondition descending="1" ref="M24:M41"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4743,11 +4780,620 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CF98E2B-B5BC-4137-BADC-315EC8730697}">
+  <dimension ref="A1:O12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O1" sqref="O1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="F1" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="G1" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="H1" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="I1" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="J1" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="K1" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="L1" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="M1" s="22" t="s">
+        <v>124</v>
+      </c>
+      <c r="N1" s="22" t="s">
+        <v>157</v>
+      </c>
+      <c r="O1" s="22"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>67</v>
+      </c>
+      <c r="F2">
+        <v>65</v>
+      </c>
+      <c r="G2">
+        <v>95</v>
+      </c>
+      <c r="H2">
+        <v>91</v>
+      </c>
+      <c r="I2">
+        <v>46</v>
+      </c>
+      <c r="J2">
+        <v>75</v>
+      </c>
+      <c r="K2">
+        <v>64</v>
+      </c>
+      <c r="L2">
+        <v>63</v>
+      </c>
+      <c r="M2">
+        <v>67</v>
+      </c>
+      <c r="N2">
+        <f>((E2/100)*30)+((G2/100)*30)+((K2/100)*30)+((L2/100)*5)+((I2/100)*5)</f>
+        <v>73.25</v>
+      </c>
+      <c r="O2">
+        <f>((F2/100)*30)+((H2/100)*30)+((K2/100)*30)+((L2/100)*5)+((I2/100)*5)</f>
+        <v>71.45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <f>A2+1</f>
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E3">
+        <v>99</v>
+      </c>
+      <c r="F3">
+        <v>94</v>
+      </c>
+      <c r="G3">
+        <v>98</v>
+      </c>
+      <c r="H3">
+        <v>74</v>
+      </c>
+      <c r="I3">
+        <v>77</v>
+      </c>
+      <c r="J3">
+        <v>64</v>
+      </c>
+      <c r="K3">
+        <v>98</v>
+      </c>
+      <c r="L3">
+        <v>34</v>
+      </c>
+      <c r="M3">
+        <v>5</v>
+      </c>
+      <c r="N3">
+        <f t="shared" ref="N3:N12" si="0">((E3/100)*30)+((G3/100)*30)+((K3/100)*30)+((L3/100)*5)+((I3/100)*5)</f>
+        <v>94.05</v>
+      </c>
+      <c r="O3">
+        <f t="shared" ref="O3:O12" si="1">((F3/100)*30)+((H3/100)*30)+((K3/100)*30)+((L3/100)*5)+((I3/100)*5)</f>
+        <v>85.35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <f t="shared" ref="A4:A12" si="2">A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>148</v>
+      </c>
+      <c r="C4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>78</v>
+      </c>
+      <c r="F4">
+        <v>82</v>
+      </c>
+      <c r="G4">
+        <v>75</v>
+      </c>
+      <c r="H4">
+        <v>45</v>
+      </c>
+      <c r="I4">
+        <v>83</v>
+      </c>
+      <c r="J4">
+        <v>68</v>
+      </c>
+      <c r="K4">
+        <v>98</v>
+      </c>
+      <c r="L4">
+        <v>80</v>
+      </c>
+      <c r="M4">
+        <v>48</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="0"/>
+        <v>83.450000000000017</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="1"/>
+        <v>75.650000000000006</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>149</v>
+      </c>
+      <c r="C5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E5">
+        <v>64</v>
+      </c>
+      <c r="F5">
+        <v>99</v>
+      </c>
+      <c r="G5">
+        <v>68</v>
+      </c>
+      <c r="H5">
+        <v>48</v>
+      </c>
+      <c r="I5">
+        <v>72</v>
+      </c>
+      <c r="J5">
+        <v>58</v>
+      </c>
+      <c r="K5">
+        <v>99</v>
+      </c>
+      <c r="L5">
+        <v>32</v>
+      </c>
+      <c r="M5">
+        <v>10</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="0"/>
+        <v>74.499999999999986</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="1"/>
+        <v>78.999999999999986</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>150</v>
+      </c>
+      <c r="C6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>67</v>
+      </c>
+      <c r="F6">
+        <v>98</v>
+      </c>
+      <c r="G6">
+        <v>64</v>
+      </c>
+      <c r="H6">
+        <v>99</v>
+      </c>
+      <c r="I6">
+        <v>46</v>
+      </c>
+      <c r="J6">
+        <v>46</v>
+      </c>
+      <c r="K6">
+        <v>69</v>
+      </c>
+      <c r="L6">
+        <v>47</v>
+      </c>
+      <c r="M6">
+        <v>5</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="0"/>
+        <v>64.650000000000006</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="1"/>
+        <v>84.449999999999989</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>151</v>
+      </c>
+      <c r="C7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>65</v>
+      </c>
+      <c r="F7">
+        <v>98</v>
+      </c>
+      <c r="G7">
+        <v>97</v>
+      </c>
+      <c r="H7">
+        <v>59</v>
+      </c>
+      <c r="I7">
+        <v>55</v>
+      </c>
+      <c r="J7">
+        <v>84</v>
+      </c>
+      <c r="K7">
+        <v>88</v>
+      </c>
+      <c r="L7">
+        <v>36</v>
+      </c>
+      <c r="M7">
+        <v>3</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="0"/>
+        <v>79.55</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="1"/>
+        <v>78.05</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>152</v>
+      </c>
+      <c r="C8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>75</v>
+      </c>
+      <c r="F8">
+        <v>85</v>
+      </c>
+      <c r="G8">
+        <v>55</v>
+      </c>
+      <c r="H8">
+        <v>75</v>
+      </c>
+      <c r="I8">
+        <v>52</v>
+      </c>
+      <c r="J8">
+        <v>38</v>
+      </c>
+      <c r="K8">
+        <v>67</v>
+      </c>
+      <c r="L8">
+        <v>83</v>
+      </c>
+      <c r="M8">
+        <v>9</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="0"/>
+        <v>65.849999999999994</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="1"/>
+        <v>74.849999999999994</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>153</v>
+      </c>
+      <c r="C9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D9" t="s">
+        <v>80</v>
+      </c>
+      <c r="E9">
+        <v>78</v>
+      </c>
+      <c r="F9">
+        <v>52</v>
+      </c>
+      <c r="G9">
+        <v>65</v>
+      </c>
+      <c r="H9">
+        <v>50</v>
+      </c>
+      <c r="I9">
+        <v>37</v>
+      </c>
+      <c r="J9">
+        <v>78</v>
+      </c>
+      <c r="K9">
+        <v>51</v>
+      </c>
+      <c r="L9">
+        <v>91</v>
+      </c>
+      <c r="M9">
+        <v>40</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="0"/>
+        <v>64.599999999999994</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="1"/>
+        <v>52.300000000000004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>154</v>
+      </c>
+      <c r="C10" t="s">
+        <v>139</v>
+      </c>
+      <c r="D10" t="s">
+        <v>81</v>
+      </c>
+      <c r="E10">
+        <v>77</v>
+      </c>
+      <c r="F10">
+        <v>77</v>
+      </c>
+      <c r="G10">
+        <v>57</v>
+      </c>
+      <c r="H10">
+        <v>43</v>
+      </c>
+      <c r="I10">
+        <v>66</v>
+      </c>
+      <c r="J10">
+        <v>43</v>
+      </c>
+      <c r="K10">
+        <v>62</v>
+      </c>
+      <c r="L10">
+        <v>91</v>
+      </c>
+      <c r="M10">
+        <v>57</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="0"/>
+        <v>66.650000000000006</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="1"/>
+        <v>62.449999999999996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>155</v>
+      </c>
+      <c r="C11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D11" t="s">
+        <v>80</v>
+      </c>
+      <c r="E11">
+        <v>87</v>
+      </c>
+      <c r="F11">
+        <v>61</v>
+      </c>
+      <c r="G11">
+        <v>58</v>
+      </c>
+      <c r="H11">
+        <v>44</v>
+      </c>
+      <c r="I11">
+        <v>61</v>
+      </c>
+      <c r="J11">
+        <v>88</v>
+      </c>
+      <c r="K11">
+        <v>78</v>
+      </c>
+      <c r="L11">
+        <v>50</v>
+      </c>
+      <c r="M11">
+        <v>11</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="0"/>
+        <v>72.45</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="1"/>
+        <v>60.45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>156</v>
+      </c>
+      <c r="C12" t="s">
+        <v>132</v>
+      </c>
+      <c r="D12" t="s">
+        <v>81</v>
+      </c>
+      <c r="E12">
+        <v>46</v>
+      </c>
+      <c r="F12">
+        <v>90</v>
+      </c>
+      <c r="G12">
+        <v>46</v>
+      </c>
+      <c r="H12">
+        <v>65</v>
+      </c>
+      <c r="I12">
+        <v>55</v>
+      </c>
+      <c r="J12">
+        <v>89</v>
+      </c>
+      <c r="K12">
+        <v>60</v>
+      </c>
+      <c r="L12">
+        <v>63</v>
+      </c>
+      <c r="M12">
+        <v>40</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="0"/>
+        <v>51.5</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="1"/>
+        <v>70.400000000000006</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8E9409E-4402-4D0B-B853-36FBBCBB5840}">
   <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5343,7 +5989,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18B86644-3852-477F-946C-1A8F21C9A9DD}">
   <dimension ref="A1:M13"/>
   <sheetViews>
@@ -5405,7 +6051,7 @@
         <v>105</v>
       </c>
       <c r="K2" s="17" t="e">
-        <f>data_lineup!#REF!/100</f>
+        <f>LAA!#REF!/100</f>
         <v>#REF!</v>
       </c>
       <c r="L2">
@@ -5442,7 +6088,7 @@
         <v>106</v>
       </c>
       <c r="K3" s="17" t="e">
-        <f>data_lineup!#REF!/100</f>
+        <f>LAA!#REF!/100</f>
         <v>#REF!</v>
       </c>
       <c r="L3">
@@ -5479,7 +6125,7 @@
         <v>107</v>
       </c>
       <c r="K4" s="17">
-        <f>data_lineup!I3/100</f>
+        <f>LAA!I3/100</f>
         <v>0.79</v>
       </c>
       <c r="L4">
@@ -5516,7 +6162,7 @@
         <v>108</v>
       </c>
       <c r="K5" s="17">
-        <f>data_lineup!J3/100</f>
+        <f>LAA!J3/100</f>
         <v>0.51</v>
       </c>
       <c r="L5">

</xml_diff>